<commit_message>
Semana 6, Clases 11 y 12
</commit_message>
<xml_diff>
--- a/content/week6/C11y12_optimizacion.xlsx
+++ b/content/week6/C11y12_optimizacion.xlsx
@@ -1,122 +1,172 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nelsonsasa07/Documents/GitHub/ua-imec2001-hc-202220/content/week6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nasalazar/Documents/GitHub/ua-imec2001-hc-202310-s1/content/week6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6BA26C-7A37-A14C-8730-6FDF8D671877}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E100431-53DF-D947-8FB2-F1793A47C6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ejemplo Lineal" sheetId="7" r:id="rId1"/>
-    <sheet name="Ejemplo No Lineal" sheetId="9" r:id="rId2"/>
+    <sheet name="Ejemplo Bomba" sheetId="10" r:id="rId1"/>
+    <sheet name="Ejemplo Lineal" sheetId="7" r:id="rId2"/>
+    <sheet name="Ejemplo No Lineal" sheetId="9" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Ejemplo Lineal'!$A$1</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$A$1</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Ejemplo Bomba'!$F$2:$F$5</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Ejemplo Lineal'!$A$1</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$A$1</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Ejemplo Lineal'!$C$10</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$C$10</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Ejemplo Lineal'!$C$11</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$C$11</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Ejemplo Lineal'!$C$12</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$C$9</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Ejemplo Lineal'!$C$13</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$C$10</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Ejemplo Lineal'!$C$14</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$C$11</definedName>
-    <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Ejemplo Lineal'!$C$9</definedName>
-    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$C$9</definedName>
-    <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Ejemplo Bomba'!$F$11</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Ejemplo Lineal'!$C$10</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$C$10</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Ejemplo Bomba'!$F$12</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Ejemplo Lineal'!$C$11</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$C$11</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Ejemplo Bomba'!$F$13</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Ejemplo Lineal'!$C$12</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$C$9</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Ejemplo Bomba'!$F$15:$F$22</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Ejemplo Lineal'!$C$13</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$C$10</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Ejemplo Lineal'!$C$14</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$C$11</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Ejemplo Lineal'!$C$9</definedName>
+    <definedName name="solver_lhs6" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$C$9</definedName>
+    <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_lin" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Ejemplo Lineal'!$A$1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$A$1</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Ejemplo Bomba'!$G$8</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Ejemplo Lineal'!$A$1</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$A$1</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel5" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel6" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Ejemplo Lineal'!$E$10</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$E$10</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Ejemplo Lineal'!$E$11</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$E$11</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Ejemplo Lineal'!$E$12</definedName>
-    <definedName name="solver_rhs3" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$E$9</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">'Ejemplo Lineal'!$E$13</definedName>
-    <definedName name="solver_rhs4" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$E$10</definedName>
-    <definedName name="solver_rhs5" localSheetId="0" hidden="1">'Ejemplo Lineal'!$E$14</definedName>
-    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$E$11</definedName>
-    <definedName name="solver_rhs6" localSheetId="0" hidden="1">'Ejemplo Lineal'!$E$9</definedName>
-    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Ejemplo No Lineal'!$E$9</definedName>
+    <definedName name="solver_rel6" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Ejemplo Bomba'!$H$11</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Ejemplo Lineal'!$E$10</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$E$10</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Ejemplo Bomba'!$H$12</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'Ejemplo Lineal'!$E$11</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$E$11</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Ejemplo Bomba'!$H$13</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">'Ejemplo Lineal'!$E$12</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$E$9</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">'Ejemplo Bomba'!$H$15:$H$22</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">'Ejemplo Lineal'!$E$13</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$E$10</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Ejemplo Lineal'!$E$14</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$E$11</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Ejemplo Lineal'!$E$9</definedName>
+    <definedName name="solver_rhs6" localSheetId="2" hidden="1">'Ejemplo No Lineal'!$E$9</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
   <si>
     <t>FUNCIÓN OBJETIVO</t>
   </si>
@@ -167,13 +217,85 @@
   </si>
   <si>
     <t xml:space="preserve"> -XY</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Rho</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>vis</t>
+  </si>
+  <si>
+    <t>H - hf</t>
+  </si>
+  <si>
+    <t>Pw</t>
+  </si>
+  <si>
+    <t>Pf</t>
+  </si>
+  <si>
+    <t>Eficiencia</t>
+  </si>
+  <si>
+    <t>10 &lt;= Q</t>
+  </si>
+  <si>
+    <t>Q &lt;= 58</t>
+  </si>
+  <si>
+    <t>200 &lt;= H</t>
+  </si>
+  <si>
+    <t>H &lt;= 655</t>
+  </si>
+  <si>
+    <t>50 &lt;= w</t>
+  </si>
+  <si>
+    <t>w &lt;= 122.5</t>
+  </si>
+  <si>
+    <t>100 &lt;= T</t>
+  </si>
+  <si>
+    <t>T &lt;= 2000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +323,33 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -216,7 +365,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -272,17 +421,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -294,19 +512,117 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -588,10 +904,375 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D812A6-9348-5841-9BC4-F36B27F94829}">
+  <dimension ref="B2:J22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="5" width="10.83203125" style="12"/>
+    <col min="6" max="6" width="11.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="12"/>
+    <col min="9" max="9" width="12.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B2" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="22">
+        <v>2</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="44">
+        <v>10.45325930786</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="25">
+        <v>1.94</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="45">
+        <v>208.689831561472</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="25">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="45">
+        <v>91.349171418359603</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="25">
+        <v>30</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="46">
+        <v>1491.4150435650599</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B6" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="16" x14ac:dyDescent="0.15">
+      <c r="B7" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="24">
+        <v>2.09E-5</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B8" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="28">
+        <f>(PI()/4)*C2^2</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="47">
+        <f>C11/C12</f>
+        <v>1.0000003191687286</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="41">
+        <f>F3-((C6*(C5/C2)*(((F2/C8)^2)/(2*C4))))</f>
+        <v>208.63825657893372</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B11" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="42">
+        <f>C3*C4*F2*C10</f>
+        <v>136239.57195394198</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="38">
+        <f>C10</f>
+        <v>208.63825657893372</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="33">
+        <v>655</v>
+      </c>
+      <c r="I11" s="34" t="b">
+        <f>F11&lt;=H11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B12" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="43">
+        <f>F4*F5</f>
+        <v>136239.5284705449</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="48">
+        <f>F2</f>
+        <v>10.45325930786</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="27">
+        <v>58</v>
+      </c>
+      <c r="I12" s="40" t="b">
+        <f>F12&lt;=H12</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="E13" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="49">
+        <f>G8</f>
+        <v>1.0000003191687286</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="36">
+        <v>1</v>
+      </c>
+      <c r="I13" s="37" t="b">
+        <f>F13&lt;=H13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="E15" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="33">
+        <v>10</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="38">
+        <f>F2</f>
+        <v>10.45325930786</v>
+      </c>
+      <c r="I15" s="34" t="b">
+        <f>F15&lt;=H15</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="E16" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="49">
+        <f>F2</f>
+        <v>10.45325930786</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="36">
+        <v>58</v>
+      </c>
+      <c r="I16" s="37" t="b">
+        <f>F16&lt;=H16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.15">
+      <c r="E17" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="33">
+        <v>200</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="38">
+        <f>F3</f>
+        <v>208.689831561472</v>
+      </c>
+      <c r="I17" s="34" t="b">
+        <f>F17&lt;=H17</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.15">
+      <c r="E18" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="49">
+        <f>F3</f>
+        <v>208.689831561472</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="36">
+        <v>655</v>
+      </c>
+      <c r="I18" s="37" t="b">
+        <f>F18&lt;=H18</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.15">
+      <c r="E19" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="33">
+        <v>50</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="38">
+        <f>F4</f>
+        <v>91.349171418359603</v>
+      </c>
+      <c r="I19" s="34" t="b">
+        <f>F19&lt;=H19</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.15">
+      <c r="E20" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="49">
+        <f>F4</f>
+        <v>91.349171418359603</v>
+      </c>
+      <c r="G20" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="36">
+        <v>122.5</v>
+      </c>
+      <c r="I20" s="37" t="b">
+        <f>F20&lt;=H20</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="5:9" x14ac:dyDescent="0.15">
+      <c r="E21" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="33">
+        <v>100</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="38">
+        <f>F5</f>
+        <v>1491.4150435650599</v>
+      </c>
+      <c r="I21" s="34" t="b">
+        <f>F21&lt;=H21</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="5:9" x14ac:dyDescent="0.15">
+      <c r="E22" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="49">
+        <f>F5</f>
+        <v>1491.4150435650599</v>
+      </c>
+      <c r="G22" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="36">
+        <v>2000</v>
+      </c>
+      <c r="I22" s="37" t="b">
+        <f>F22&lt;=H22</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95BF774-3A22-1F4D-836A-49C30C79515D}">
   <dimension ref="B2:F15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -602,23 +1283,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="2:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="2:6" ht="16" x14ac:dyDescent="0.15">
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
       <c r="C6" s="6" t="s">
@@ -627,14 +1308,14 @@
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="8" spans="2:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="C8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="C8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
@@ -737,7 +1418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C00B593E-CD0C-0E44-8FD3-D4EDB2E71391}">
   <dimension ref="B2:F12"/>
   <sheetViews>
@@ -752,23 +1433,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="2:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="2:6" ht="16" x14ac:dyDescent="0.15">
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
       <c r="C6" s="6" t="s">
@@ -777,14 +1458,14 @@
       <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="8" spans="2:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="C8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="C8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">

</xml_diff>